<commit_message>
Data until 45deg beam steer. Phase and Amplitude need be reversed for plots.
</commit_message>
<xml_diff>
--- a/matlab/experiment/25Aug/30deg/AAA_4.xlsx
+++ b/matlab/experiment/25Aug/30deg/AAA_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltd\OneDrive\Documents\2021\semester2\thesis-2021\matlab\experiment\25Aug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltd\OneDrive\Documents\2021\semester2\thesis-2021\matlab\experiment\25Aug\30deg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470867F1-E0F9-437C-B090-DD0CE3B20DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67974DBB-9485-4E74-901F-453EA116A230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D543AE69-3697-4970-A4AF-1CE2B847E7B0}"/>
+    <workbookView xWindow="-1452" yWindow="1488" windowWidth="19812" windowHeight="11616" xr2:uid="{D543AE69-3697-4970-A4AF-1CE2B847E7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
   <si>
     <t>Spacing</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Amplitude</t>
+  </si>
+  <si>
+    <t>convert to db scale</t>
   </si>
 </sst>
 </file>
@@ -6261,7 +6264,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-ZA" sz="1100"/>
-            <a:t>Phase optimasation</a:t>
+            <a:t>Phase optimization</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6324,7 +6327,23 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-ZA" sz="1100"/>
-            <a:t>Amplitude optimasation </a:t>
+            <a:t>Amplitude </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>optimization</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100"/>
+            <a:t> </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6772,14 +6791,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61969A2-35CE-4EA2-A663-E2E34A29B945}">
-  <dimension ref="B21:AO23"/>
+  <dimension ref="B5:AS23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U88" sqref="U88"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="5" spans="45:45" x14ac:dyDescent="0.3">
+      <c r="AS5" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>0</v>
@@ -7039,8 +7063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BDFD6C7-89D8-45F8-95EC-6103B8B446D2}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:E50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7904,8 +7928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54132F2-7160-45FF-B5D3-E2F3B79342E1}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:F50"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8919,7 +8943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206B63A3-D08A-412E-B9B7-58B12816A56B}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A50" sqref="A50:F50"/>
     </sheetView>
   </sheetViews>
@@ -9934,8 +9958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4C447F-9126-4D03-82C9-16B022A11520}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10200,7 +10224,7 @@
   <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10464,8 +10488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509FD69F-2FB7-4CD8-A327-C0B62579EC4E}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A48:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>